<commit_message>
reload modulos cierre cuentas por cobrar
</commit_message>
<xml_diff>
--- a/recursos/FALTANTES CONSORCIO_10112022.xlsx
+++ b/recursos/FALTANTES CONSORCIO_10112022.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevFiles\xampps\7.0.32\htdocs\consorcio_test\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757DF61A-E58F-4AE0-AEF4-22D401E39D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2400"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -254,7 +244,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -651,11 +641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1107,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="C12:D26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C12:D26">
     <sortCondition ref="D12:D26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>